<commit_message>
Update to Beam 364 UFF
</commit_message>
<xml_diff>
--- a/beams-test.xlsx
+++ b/beams-test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhampleman/Katalon Studio/Exede_Beam_Tests_v2.1 copy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhampleman/jenkins-beam-tests-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807CD50D-4277-CC4E-A540-1F971FC669A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4B7E88-EC01-4C42-8200-2348A8234AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="73100" yWindow="-16100" windowWidth="34680" windowHeight="20560" xr2:uid="{CA3EBB14-1765-FE45-ABE3-2D37D1D7B544}"/>
+    <workbookView xWindow="34180" yWindow="-16100" windowWidth="34680" windowHeight="20040" xr2:uid="{CA3EBB14-1765-FE45-ABE3-2D37D1D7B544}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1724,7 +1724,7 @@
   <dimension ref="A1:M145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="F129" sqref="F129"/>
+      <selection activeCell="K130" sqref="K130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5746,7 +5746,7 @@
         <v>95932</v>
       </c>
       <c r="K129" s="6">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="L129" s="6"/>
       <c r="M129" s="6"/>

</xml_diff>